<commit_message>
Discrepancy in visualizaing hexBins happens after scale_x/y_continuous
</commit_message>
<xml_diff>
--- a/ShinyPlotly/Hex/HexPairs/app2-CurveNumber.xlsx
+++ b/ShinyPlotly/Hex/HexPairs/app2-CurveNumber.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>count</t>
   </si>
@@ -67,6 +67,45 @@
   </si>
   <si>
     <t>DE-15</t>
+  </si>
+  <si>
+    <t>AB</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>AD</t>
+  </si>
+  <si>
+    <t>AE</t>
+  </si>
+  <si>
+    <t>BC</t>
+  </si>
+  <si>
+    <t>BD</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>CD</t>
+  </si>
+  <si>
+    <t>CE</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>See before pS</t>
+  </si>
+  <si>
+    <t>See after pS</t>
+  </si>
+  <si>
+    <t>hexdf</t>
   </si>
 </sst>
 </file>
@@ -129,8 +168,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -154,10 +195,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -168,6 +209,7 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -178,6 +220,7 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -507,11 +550,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D164"/>
+  <dimension ref="A1:D163"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A100" sqref="A100"/>
+      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C170" sqref="C170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -531,7 +574,7 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D2">
@@ -671,7 +714,7 @@
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D15">
@@ -811,7 +854,7 @@
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D28">
@@ -951,7 +994,7 @@
       </c>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D41">
@@ -1138,7 +1181,7 @@
       </c>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" s="2" t="s">
+      <c r="A58" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D58" t="s">
@@ -1311,7 +1354,7 @@
       </c>
     </row>
     <row r="74" spans="1:4">
-      <c r="A74" s="2" t="s">
+      <c r="A74" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D74">
@@ -1462,7 +1505,7 @@
       </c>
     </row>
     <row r="88" spans="1:4">
-      <c r="A88" s="2" t="s">
+      <c r="A88" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D88">
@@ -1605,7 +1648,7 @@
       </c>
     </row>
     <row r="101" spans="1:4">
-      <c r="A101" s="2" t="s">
+      <c r="A101" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D101" t="s">
@@ -1789,7 +1832,7 @@
       </c>
     </row>
     <row r="118" spans="1:4">
-      <c r="A118" s="2" t="s">
+      <c r="A118" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D118">
@@ -1987,7 +2030,7 @@
       </c>
     </row>
     <row r="136" spans="1:4">
-      <c r="A136" s="2" t="s">
+      <c r="A136" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D136" t="s">
@@ -2085,7 +2128,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="145" spans="1:3">
+    <row r="145" spans="1:4">
       <c r="A145">
         <v>5</v>
       </c>
@@ -2096,7 +2139,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="146" spans="1:3">
+    <row r="146" spans="1:4">
       <c r="A146">
         <v>6</v>
       </c>
@@ -2107,7 +2150,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="147" spans="1:3">
+    <row r="147" spans="1:4">
       <c r="A147">
         <v>10</v>
       </c>
@@ -2118,7 +2161,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="148" spans="1:3">
+    <row r="148" spans="1:4">
       <c r="A148">
         <v>11</v>
       </c>
@@ -2129,7 +2172,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="149" spans="1:3">
+    <row r="149" spans="1:4">
       <c r="A149">
         <v>11</v>
       </c>
@@ -2140,7 +2183,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="150" spans="1:3">
+    <row r="150" spans="1:4">
       <c r="A150">
         <v>16</v>
       </c>
@@ -2151,7 +2194,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="151" spans="1:3">
+    <row r="151" spans="1:4">
       <c r="A151">
         <v>26</v>
       </c>
@@ -2162,60 +2205,155 @@
         <v>162</v>
       </c>
     </row>
-    <row r="154" spans="1:3">
-      <c r="A154">
+    <row r="153" spans="1:4">
+      <c r="B153" t="s">
+        <v>27</v>
+      </c>
+      <c r="C153" t="s">
+        <v>26</v>
+      </c>
+      <c r="D153" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4">
+      <c r="A154" t="s">
+        <v>16</v>
+      </c>
+      <c r="B154">
         <v>12</v>
       </c>
-    </row>
-    <row r="155" spans="1:3">
-      <c r="A155">
+      <c r="C154">
         <v>12</v>
       </c>
-    </row>
-    <row r="156" spans="1:3">
-      <c r="A156">
+      <c r="D154">
         <v>12</v>
       </c>
     </row>
-    <row r="157" spans="1:3">
-      <c r="A157">
+    <row r="155" spans="1:4">
+      <c r="A155" t="s">
+        <v>17</v>
+      </c>
+      <c r="B155">
+        <v>12</v>
+      </c>
+      <c r="C155">
+        <v>12</v>
+      </c>
+      <c r="D155">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4">
+      <c r="A156" t="s">
+        <v>18</v>
+      </c>
+      <c r="B156">
+        <v>12</v>
+      </c>
+      <c r="C156">
+        <v>12</v>
+      </c>
+      <c r="D156">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4">
+      <c r="A157" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B157" s="2">
         <v>16</v>
       </c>
-    </row>
-    <row r="158" spans="1:3">
-      <c r="A158">
+      <c r="C157" s="2">
+        <v>17</v>
+      </c>
+      <c r="D157">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4">
+      <c r="A158" t="s">
+        <v>20</v>
+      </c>
+      <c r="B158">
         <v>15</v>
       </c>
-    </row>
-    <row r="159" spans="1:3">
-      <c r="A159">
+      <c r="C158">
+        <v>15</v>
+      </c>
+      <c r="D158">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4">
+      <c r="A159" t="s">
+        <v>21</v>
+      </c>
+      <c r="B159">
         <v>13</v>
       </c>
-    </row>
-    <row r="160" spans="1:3">
-      <c r="A160">
+      <c r="C159">
+        <v>13</v>
+      </c>
+      <c r="D159">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4">
+      <c r="A160" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B160" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="161" spans="1:1">
-      <c r="A161">
+      <c r="C160" s="2">
+        <v>13</v>
+      </c>
+      <c r="D160">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4">
+      <c r="A161" t="s">
+        <v>23</v>
+      </c>
+      <c r="B161">
         <v>16</v>
       </c>
-    </row>
-    <row r="162" spans="1:1">
-      <c r="A162">
+      <c r="C161">
+        <v>16</v>
+      </c>
+      <c r="D161">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4">
+      <c r="A162" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B162" s="2">
         <v>17</v>
       </c>
-    </row>
-    <row r="163" spans="1:1">
-      <c r="A163">
+      <c r="C162" s="2">
+        <v>18</v>
+      </c>
+      <c r="D162">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4">
+      <c r="A163" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B163" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="164" spans="1:1">
-      <c r="A164" s="1">
-        <f>SUM(A154:A163)</f>
-        <v>140</v>
+      <c r="C163" s="2">
+        <v>16</v>
+      </c>
+      <c r="D163">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Confidence intervals for geom_abline
</commit_message>
<xml_diff>
--- a/ShinyPlotly/Hex/HexPairs/app2-CurveNumber.xlsx
+++ b/ShinyPlotly/Hex/HexPairs/app2-CurveNumber.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="17140" yWindow="0" windowWidth="8000" windowHeight="14580" tabRatio="500"/>
+    <workbookView xWindow="11600" yWindow="0" windowWidth="10980" windowHeight="14580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>count</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t>hexdf</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
   </si>
 </sst>
 </file>
@@ -193,10 +199,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -550,11 +557,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D163"/>
+  <dimension ref="A1:G163"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C170" sqref="C170"/>
+      <pane ySplit="1" topLeftCell="A141" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A163" sqref="A163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2128,7 +2135,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="145" spans="1:4">
+    <row r="145" spans="1:7">
       <c r="A145">
         <v>5</v>
       </c>
@@ -2139,7 +2146,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="146" spans="1:4">
+    <row r="146" spans="1:7">
       <c r="A146">
         <v>6</v>
       </c>
@@ -2150,7 +2157,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="147" spans="1:4">
+    <row r="147" spans="1:7">
       <c r="A147">
         <v>10</v>
       </c>
@@ -2161,7 +2168,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="148" spans="1:4">
+    <row r="148" spans="1:7">
       <c r="A148">
         <v>11</v>
       </c>
@@ -2172,7 +2179,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="149" spans="1:4">
+    <row r="149" spans="1:7">
       <c r="A149">
         <v>11</v>
       </c>
@@ -2183,7 +2190,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="150" spans="1:4">
+    <row r="150" spans="1:7">
       <c r="A150">
         <v>16</v>
       </c>
@@ -2194,7 +2201,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="151" spans="1:4">
+    <row r="151" spans="1:7">
       <c r="A151">
         <v>26</v>
       </c>
@@ -2205,7 +2212,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="153" spans="1:4">
+    <row r="153" spans="1:7">
       <c r="B153" t="s">
         <v>27</v>
       </c>
@@ -2215,8 +2222,14 @@
       <c r="D153" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="154" spans="1:4">
+      <c r="E153" t="s">
+        <v>29</v>
+      </c>
+      <c r="F153" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7">
       <c r="A154" t="s">
         <v>16</v>
       </c>
@@ -2229,8 +2242,15 @@
       <c r="D154">
         <v>12</v>
       </c>
-    </row>
-    <row r="155" spans="1:4">
+      <c r="E154" s="3">
+        <v>1</v>
+      </c>
+      <c r="F154" s="3">
+        <v>12</v>
+      </c>
+      <c r="G154" s="3"/>
+    </row>
+    <row r="155" spans="1:7">
       <c r="A155" t="s">
         <v>17</v>
       </c>
@@ -2243,8 +2263,15 @@
       <c r="D155">
         <v>12</v>
       </c>
-    </row>
-    <row r="156" spans="1:4">
+      <c r="E155" s="3">
+        <v>14</v>
+      </c>
+      <c r="F155" s="3">
+        <v>25</v>
+      </c>
+      <c r="G155" s="3"/>
+    </row>
+    <row r="156" spans="1:7">
       <c r="A156" t="s">
         <v>18</v>
       </c>
@@ -2257,8 +2284,15 @@
       <c r="D156">
         <v>12</v>
       </c>
-    </row>
-    <row r="157" spans="1:4">
+      <c r="E156" s="3">
+        <v>27</v>
+      </c>
+      <c r="F156" s="3">
+        <v>38</v>
+      </c>
+      <c r="G156" s="3"/>
+    </row>
+    <row r="157" spans="1:7">
       <c r="A157" s="2" t="s">
         <v>19</v>
       </c>
@@ -2271,8 +2305,15 @@
       <c r="D157">
         <v>17</v>
       </c>
-    </row>
-    <row r="158" spans="1:4">
+      <c r="E157" s="3">
+        <v>40</v>
+      </c>
+      <c r="F157" s="3">
+        <v>56</v>
+      </c>
+      <c r="G157" s="3"/>
+    </row>
+    <row r="158" spans="1:7">
       <c r="A158" t="s">
         <v>20</v>
       </c>
@@ -2285,8 +2326,15 @@
       <c r="D158">
         <v>15</v>
       </c>
-    </row>
-    <row r="159" spans="1:4">
+      <c r="E158" s="3">
+        <v>60</v>
+      </c>
+      <c r="F158" s="3">
+        <v>74</v>
+      </c>
+      <c r="G158" s="3"/>
+    </row>
+    <row r="159" spans="1:7">
       <c r="A159" t="s">
         <v>21</v>
       </c>
@@ -2299,8 +2347,15 @@
       <c r="D159">
         <v>13</v>
       </c>
-    </row>
-    <row r="160" spans="1:4">
+      <c r="E159" s="3">
+        <v>76</v>
+      </c>
+      <c r="F159" s="3">
+        <v>88</v>
+      </c>
+      <c r="G159" s="3"/>
+    </row>
+    <row r="160" spans="1:7">
       <c r="A160" s="2" t="s">
         <v>22</v>
       </c>
@@ -2313,8 +2368,15 @@
       <c r="D160">
         <v>13</v>
       </c>
-    </row>
-    <row r="161" spans="1:4">
+      <c r="E160" s="3">
+        <v>90</v>
+      </c>
+      <c r="F160" s="3">
+        <v>102</v>
+      </c>
+      <c r="G160" s="3"/>
+    </row>
+    <row r="161" spans="1:7">
       <c r="A161" t="s">
         <v>23</v>
       </c>
@@ -2327,8 +2389,15 @@
       <c r="D161">
         <v>16</v>
       </c>
-    </row>
-    <row r="162" spans="1:4">
+      <c r="E161" s="3">
+        <v>107</v>
+      </c>
+      <c r="F161" s="3">
+        <v>122</v>
+      </c>
+      <c r="G161" s="3"/>
+    </row>
+    <row r="162" spans="1:7">
       <c r="A162" s="2" t="s">
         <v>24</v>
       </c>
@@ -2341,8 +2410,15 @@
       <c r="D162">
         <v>18</v>
       </c>
-    </row>
-    <row r="163" spans="1:4">
+      <c r="E162" s="3">
+        <v>124</v>
+      </c>
+      <c r="F162" s="3">
+        <v>141</v>
+      </c>
+      <c r="G162" s="3"/>
+    </row>
+    <row r="163" spans="1:7">
       <c r="A163" s="2" t="s">
         <v>25</v>
       </c>
@@ -2355,6 +2431,13 @@
       <c r="D163">
         <v>16</v>
       </c>
+      <c r="E163" s="3">
+        <v>147</v>
+      </c>
+      <c r="F163" s="3">
+        <v>162</v>
+      </c>
+      <c r="G163" s="3"/>
     </row>
   </sheetData>
   <sortState ref="A136:C150">

</xml_diff>

<commit_message>
creating attribute on h@cID
</commit_message>
<xml_diff>
--- a/ShinyPlotly/Hex/HexPairs/app2-CurveNumber.xlsx
+++ b/ShinyPlotly/Hex/HexPairs/app2-CurveNumber.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11600" yWindow="0" windowWidth="10980" windowHeight="14580" tabRatio="500"/>
+    <workbookView xWindow="19580" yWindow="0" windowWidth="8000" windowHeight="14400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -560,8 +560,8 @@
   <dimension ref="A1:G163"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A141" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A163" sqref="A163"/>
+      <pane ySplit="1" topLeftCell="A138" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D169" sqref="D169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>